<commit_message>
Updated genBankAssembly accession with NCBI Assembly accession.  Updated some biosample accessions.
</commit_message>
<xml_diff>
--- a/datasets/Escherichia_coli_1405WAEXK-1.xlsx
+++ b/datasets/Escherichia_coli_1405WAEXK-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\data.biotech.cdc.gov\home\src\datasets\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\WGS-standards-and-analysis\devel\datasets.git\trunk\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -164,9 +164,6 @@
     <t>1405WAEXK-1</t>
   </si>
   <si>
-    <t>JASV01000000</t>
-  </si>
-  <si>
     <t>2011C-3609</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855</t>
+  </si>
+  <si>
+    <t>GCA_000703365.1</t>
   </si>
 </sst>
 </file>
@@ -604,14 +604,16 @@
       <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="17.85546875" style="2"/>
     <col min="5" max="5" width="17.85546875" style="3"/>
-    <col min="6" max="16384" width="17.85546875" style="2"/>
+    <col min="6" max="7" width="17.85546875" style="2"/>
+    <col min="8" max="8" width="22.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="17.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -640,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -648,7 +650,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -697,19 +699,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>45</v>
@@ -718,13 +720,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,7 +737,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>36</v>
@@ -750,13 +752,13 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -767,7 +769,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>37</v>
@@ -782,13 +784,13 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -799,7 +801,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>38</v>
@@ -814,13 +816,13 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -831,13 +833,13 @@
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>45</v>
@@ -846,30 +848,30 @@
         <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>45</v>
@@ -878,30 +880,30 @@
         <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>45</v>
@@ -910,30 +912,30 @@
         <v>0</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>45</v>
@@ -942,30 +944,30 @@
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>45</v>
@@ -974,30 +976,30 @@
         <v>0</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>45</v>
@@ -1006,16 +1008,19 @@
         <v>0</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A9:J18">
+    <sortCondition ref="A8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
E. coli tree of life link
</commit_message>
<xml_diff>
--- a/datasets/Escherichia_coli_1405WAEXK-1.xlsx
+++ b/datasets/Escherichia_coli_1405WAEXK-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\WGS-standards-and-analysis\devel\datasets.git\trunk\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\data.biotech.cdc.gov\home\src\datasets\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -179,9 +179,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/WGS-standards-and-analysis/datasets/master/datasets/trees/Escherichia_coli_1405WAEXK-1.dnd</t>
-  </si>
-  <si>
     <t>0264dc57015100fe41a9a9167145439eb383ea8216b49785a09ce5157293e080</t>
   </si>
   <si>
@@ -240,13 +237,16 @@
   </si>
   <si>
     <t>GCA_000703365.1</t>
+  </si>
+  <si>
+    <t>http://api.opentreeoflife.org/v2/study/ot_301/tree/tree3.tre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +265,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,10 +310,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -318,8 +327,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,7 +615,7 @@
       <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -641,8 +652,8 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>51</v>
+      <c r="B4" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -705,7 +716,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>50</v>
@@ -720,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>50</v>
@@ -755,10 +766,10 @@
         <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -787,10 +798,10 @@
         <v>50</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -819,10 +830,10 @@
         <v>50</v>
       </c>
       <c r="I12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -851,10 +862,10 @@
         <v>50</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -883,10 +894,10 @@
         <v>50</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -915,10 +926,10 @@
         <v>50</v>
       </c>
       <c r="I15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -947,10 +958,10 @@
         <v>50</v>
       </c>
       <c r="I16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -979,10 +990,10 @@
         <v>50</v>
       </c>
       <c r="I17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1011,17 +1022,20 @@
         <v>50</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A9:J18">
     <sortCondition ref="A8"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>